<commit_message>
FEAT: add fetching from multiple local files
</commit_message>
<xml_diff>
--- a/output/data.xlsx
+++ b/output/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,45 +483,92 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>67890</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Charles Darwin</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>The Descent of Man</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>and Selection in Relation to Sex</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Berlin</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>John Murray</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1871</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Second edition</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>ALT-123</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>12345</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>Charles Darwin</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>On the Origin of Species</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>by Means of Natural Selection</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>London; Paris</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>NaN</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>1859</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>First edition</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>ALT-999</t>
         </is>

</xml_diff>

<commit_message>
FIX: fix materialization of global entities
</commit_message>
<xml_diff>
--- a/output/data.xlsx
+++ b/output/data.xlsx
@@ -553,11 +553,7 @@
           <t>London; Paris</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
           <t>1859</t>

</xml_diff>

<commit_message>
FIX: experiment with extraction from internet archive, found some bugs to solve in cleaning
</commit_message>
<xml_diff>
--- a/output/data.xlsx
+++ b/output/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,92 +483,352 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>67890</t>
+          <t>1000028</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Charles Darwin</t>
+          <t>Abercrombie, John</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>The Descent of Man</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>and Selection in Relation to Sex</t>
-        </is>
-      </c>
+          <t>Inquiries concerning the intellectual powers and the investigation of truth.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Berlin</t>
+          <t>London :</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>John Murray</t>
+          <t>John Murray,</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>1871</t>
+          <t>1838</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Second edition</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>ALT-123</t>
-        </is>
-      </c>
+          <t>Location: Cambridge.; Identifier: Abercrombie1838wa66W.; Public number: 0001.</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>12345</t>
+          <t>1000029</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Charles Darwin</t>
+          <t>Darwin, Charles</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>On the Origin of Species</t>
+          <t>Inquiries concerning the intellectual powers and the investigation of truth. :</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>by Means of Natural Selection</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>London; Paris</t>
-        </is>
-      </c>
+          <t>[Supplementary material in Charles Darwin's copy].</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>1859</t>
-        </is>
-      </c>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
-          <t>First edition</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>ALT-999</t>
-        </is>
-      </c>
+          <t>Identifier: Abercrombie1838wa66W_MS.</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1000159</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Agassiz, Louis</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Lake Superior: its character, vegetation, and animals, compared with those of other similar regions.</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Boston :</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Gould, Kendall &amp; Lincoln,</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1850</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Inscription.; Location: Cambridge.; Identifier: Agassiz1850up52I.; Public number: 0017.</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1000160</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Darwin, Charles</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Lake Superior: its character, vegetation, and animals, compared with those of other similar regions. :</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>[Supplementary material in Charles Darwin's copy].</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Identifier: Agassiz1850up52I_MS.</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1000223</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Agassiz, Louis</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Contributions to the natural history of the United States of North America.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>[s.n.] :</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>,</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>n.d..</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Inscription.; Essay on classification.; Location: Cambridge.; Identifier: Agassiz2006ft69Y.; Public number: 0015.</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>1000224</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Darwin, Charles</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Contributions to the natural history of the United States of North America. :</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>[Supplementary material in Charles Darwin's copy].</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Identifier: Agassiz2006ft69Y_MS.</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>1000345</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Barker-Webb, Philip</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Histoire naturelle des Îles Canaries.</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Paris :</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Béthune,</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>1840</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Location: Cambridge.; Identifier: Barker-Webb1840yf41S.; Public number: 0063.</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>1000346</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Darwin, Charles</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Histoire naturelle des Îles Canaries. :</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>[Supplementary material in Charles Darwin's copy].</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Identifier: Barker-Webb1840yf41S_MS.</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>1000128</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Bechstein, Johann Matthäus</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Naturgeschichte der Stubenvögel.</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Halle :</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Hennemann,</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>1840</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Signature.; Location: Cambridge.; Identifier: Bechstein1840ob74D.; Public number: 0083.</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>1000129</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Darwin, Charles</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Naturgeschichte der Stubenvögel. :</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>[Supplementary material in Charles Darwin's copy].</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Identifier: Bechstein1840ob74D_MS.</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
FIX: experiment with internetarchive extractor
</commit_message>
<xml_diff>
--- a/output/data.xlsx
+++ b/output/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,18 +493,18 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Inquiries concerning the intellectual powers and the investigation of truth.</t>
+          <t>Inquiries concerning the intellectual powers and the investigation of truth</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>London :</t>
+          <t>London</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>John Murray,</t>
+          <t>John Murray</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -532,12 +532,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Inquiries concerning the intellectual powers and the investigation of truth. :</t>
+          <t>Inquiries concerning the intellectual powers and the investigation of truth</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[Supplementary material in Charles Darwin's copy].</t>
+          <t>[Supplementary material in Charles Darwin's copy]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -563,18 +563,18 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Lake Superior: its character, vegetation, and animals, compared with those of other similar regions.</t>
+          <t>Lake Superior: its character, vegetation, and animals, compared with those of other similar regions</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Boston :</t>
+          <t>Boston</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Gould, Kendall &amp; Lincoln,</t>
+          <t>Gould, Kendall &amp; Lincoln</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -602,12 +602,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Lake Superior: its character, vegetation, and animals, compared with those of other similar regions. :</t>
+          <t>Lake Superior: its character, vegetation, and animals, compared with those of other similar regions</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[Supplementary material in Charles Darwin's copy].</t>
+          <t>[Supplementary material in Charles Darwin's copy]</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -633,25 +633,13 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Contributions to the natural history of the United States of North America.</t>
+          <t>Contributions to the natural history of the United States of North America</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>[s.n.] :</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>,</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>n.d..</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>Inscription.; Essay on classification.; Location: Cambridge.; Identifier: Agassiz2006ft69Y.; Public number: 0015.</t>
@@ -672,12 +660,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Contributions to the natural history of the United States of North America. :</t>
+          <t>Contributions to the natural history of the United States of North America</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>[Supplementary material in Charles Darwin's copy].</t>
+          <t>[Supplementary material in Charles Darwin's copy]</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -703,18 +691,18 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Histoire naturelle des Îles Canaries.</t>
+          <t>Histoire naturelle des Îles Canaries</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Paris :</t>
+          <t>Paris</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Béthune,</t>
+          <t>Béthune</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -742,12 +730,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Histoire naturelle des Îles Canaries. :</t>
+          <t>Histoire naturelle des Îles Canaries</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>[Supplementary material in Charles Darwin's copy].</t>
+          <t>[Supplementary material in Charles Darwin's copy]</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -773,18 +761,18 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Naturgeschichte der Stubenvögel.</t>
+          <t>Naturgeschichte der Stubenvögel</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Halle :</t>
+          <t>Halle</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Hennemann,</t>
+          <t>Hennemann</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -812,12 +800,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Naturgeschichte der Stubenvögel. :</t>
+          <t>Naturgeschichte der Stubenvögel</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>[Supplementary material in Charles Darwin's copy].</t>
+          <t>[Supplementary material in Charles Darwin's copy]</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -830,6 +818,185 @@
       </c>
       <c r="I11" t="inlineStr"/>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>1000241</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Bell, Charles</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>The anatomy and philosophy of expression</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>John Murray</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>1844</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Signature E. Darwin 1844 to Ch. Darwin Nov. 28 1866.; Location: Cambridge.; Identifier: Bell1844nu34M.; Public number: 0085.</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>1000242</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Darwin, Charles</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>The anatomy and philosophy of expression</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>[Supplementary material in Charles Darwin's copy]</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Identifier: Bell1844nu34M_MS.</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>1000116</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Bernhardi, Johann Jacob</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>über den Begriff der Pflanzenart und seine Anwendung</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Erfurt</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Friedrich Wilhelm Otto</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>1834</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Location: Cambridge.; Identifier: Bernhardi1834ez86I.; Public number: 0098.</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>1000117</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Darwin, Charles</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>über den Begriff der Pflanzenart und seine Anwendung</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>[Supplementary material in Charles Darwin's copy]</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Identifier: Bernhardi1834ez86I_MS.</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>1000141</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Boitard, Pierre</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Les Pigeons de volière et de colombier, ou Histoire naturelle des pigeons domestiques</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Paris</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Audot &amp; Corbié</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>1824</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Pre-Beagle.; Location: Cambridge.; Identifier: Boitard1824jp50S.; Public number: 0118.</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>